<commit_message>
Modified Connections_Table for Keypad
</commit_message>
<xml_diff>
--- a/Connections_Table.xlsx
+++ b/Connections_Table.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="37">
   <si>
     <t>Expansion Board J11</t>
   </si>
@@ -111,6 +111,30 @@
   </si>
   <si>
     <t>Expansion Board J10 (11)</t>
+  </si>
+  <si>
+    <t>4x3 Keypad</t>
+  </si>
+  <si>
+    <t>Expansion Board J10 (15)</t>
+  </si>
+  <si>
+    <t>Expansion Board J10 (17)</t>
+  </si>
+  <si>
+    <t>Expansion Board J11 (6)</t>
+  </si>
+  <si>
+    <t>Expansion Board J11 (8)</t>
+  </si>
+  <si>
+    <t>Expansion Board J11 (10)</t>
+  </si>
+  <si>
+    <t>Row</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Column </t>
   </si>
 </sst>
 </file>
@@ -465,15 +489,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K28"/>
+  <dimension ref="A1:O28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M1" sqref="M1"/>
+      <selection activeCell="M19" sqref="M19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="10" max="10" width="23" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="23" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="10.42578125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -483,8 +514,11 @@
       <c r="I1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -512,8 +546,17 @@
       <c r="K2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M2" t="s">
+        <v>6</v>
+      </c>
+      <c r="N2" t="s">
+        <v>4</v>
+      </c>
+      <c r="O2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>4</v>
       </c>
@@ -536,8 +579,17 @@
       <c r="K3" s="2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M3">
+        <v>1</v>
+      </c>
+      <c r="N3" t="s">
+        <v>33</v>
+      </c>
+      <c r="O3" s="4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4">
         <f>A3+2</f>
         <v>6</v>
@@ -567,8 +619,17 @@
       <c r="K4" s="3" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M4">
+        <v>2</v>
+      </c>
+      <c r="N4" t="s">
+        <v>30</v>
+      </c>
+      <c r="O4" s="6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5">
         <f t="shared" ref="A5:A24" si="0">A4+2</f>
         <v>8</v>
@@ -598,8 +659,17 @@
       <c r="K5" s="5" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M5">
+        <v>3</v>
+      </c>
+      <c r="N5" t="s">
+        <v>32</v>
+      </c>
+      <c r="O5" s="4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -629,8 +699,17 @@
       <c r="K6" s="6" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M6">
+        <v>4</v>
+      </c>
+      <c r="N6" t="s">
+        <v>15</v>
+      </c>
+      <c r="O6" s="6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7">
         <f t="shared" si="0"/>
         <v>12</v>
@@ -660,8 +739,17 @@
       <c r="K7" s="5" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M7">
+        <v>5</v>
+      </c>
+      <c r="N7" t="s">
+        <v>34</v>
+      </c>
+      <c r="O7" s="4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8">
         <f t="shared" si="0"/>
         <v>14</v>
@@ -691,8 +779,17 @@
       <c r="K8" s="6" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M8">
+        <v>6</v>
+      </c>
+      <c r="N8" t="s">
+        <v>19</v>
+      </c>
+      <c r="O8" s="6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9">
         <f t="shared" si="0"/>
         <v>16</v>
@@ -722,8 +819,17 @@
       <c r="K9" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M9">
+        <v>7</v>
+      </c>
+      <c r="N9" t="s">
+        <v>31</v>
+      </c>
+      <c r="O9" s="6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10">
         <f t="shared" si="0"/>
         <v>18</v>
@@ -754,7 +860,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11">
         <f t="shared" si="0"/>
         <v>20</v>
@@ -785,7 +891,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12">
         <f t="shared" si="0"/>
         <v>22</v>
@@ -815,8 +921,14 @@
       <c r="K12" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="N12" t="s">
+        <v>35</v>
+      </c>
+      <c r="O12" s="6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13">
         <f t="shared" si="0"/>
         <v>24</v>
@@ -846,8 +958,14 @@
       <c r="K13" s="4" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="N13" t="s">
+        <v>36</v>
+      </c>
+      <c r="O13" s="4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14">
         <f t="shared" si="0"/>
         <v>26</v>
@@ -878,7 +996,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15">
         <f t="shared" si="0"/>
         <v>28</v>
@@ -909,7 +1027,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16">
         <f t="shared" si="0"/>
         <v>30</v>

</xml_diff>

<commit_message>
Passwords now correctly being compared, 'bad', 'good',etc not displaying long enough though
</commit_message>
<xml_diff>
--- a/Connections_Table.xlsx
+++ b/Connections_Table.xlsx
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="p1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="162912"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="43">
   <si>
     <t>Expansion Board J11</t>
   </si>
@@ -116,12 +116,6 @@
     <t>4x3 Keypad</t>
   </si>
   <si>
-    <t>Expansion Board J10 (15)</t>
-  </si>
-  <si>
-    <t>Expansion Board J10 (17)</t>
-  </si>
-  <si>
     <t>Expansion Board J11 (6)</t>
   </si>
   <si>
@@ -135,12 +129,24 @@
   </si>
   <si>
     <t xml:space="preserve">Column </t>
+  </si>
+  <si>
+    <t>Expansion Board J11 (5)</t>
+  </si>
+  <si>
+    <t>Expansion Board J11 (7)</t>
+  </si>
+  <si>
+    <t>Expansion Board J11 (11)</t>
+  </si>
+  <si>
+    <t>Expansion Board J11 (9)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -491,11 +497,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M19" sqref="M19"/>
+    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
+      <selection activeCell="N8" sqref="N8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="10" max="10" width="23" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="10.42578125" bestFit="1" customWidth="1"/>
@@ -504,7 +510,7 @@
     <col min="15" max="15" width="10.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -518,7 +524,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -556,7 +562,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>4</v>
       </c>
@@ -583,13 +589,13 @@
         <v>1</v>
       </c>
       <c r="N3" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="O3" s="4" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A4">
         <f>A3+2</f>
         <v>6</v>
@@ -623,13 +629,13 @@
         <v>2</v>
       </c>
       <c r="N4" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="O4" s="6" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A5">
         <f t="shared" ref="A5:A24" si="0">A4+2</f>
         <v>8</v>
@@ -663,13 +669,13 @@
         <v>3</v>
       </c>
       <c r="N5" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="O5" s="4" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A6">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -703,13 +709,13 @@
         <v>4</v>
       </c>
       <c r="N6" t="s">
-        <v>15</v>
+        <v>37</v>
       </c>
       <c r="O6" s="6" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A7">
         <f t="shared" si="0"/>
         <v>12</v>
@@ -743,13 +749,13 @@
         <v>5</v>
       </c>
       <c r="N7" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="O7" s="4" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A8">
         <f t="shared" si="0"/>
         <v>14</v>
@@ -783,13 +789,13 @@
         <v>6</v>
       </c>
       <c r="N8" t="s">
-        <v>19</v>
+        <v>38</v>
       </c>
       <c r="O8" s="6" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A9">
         <f t="shared" si="0"/>
         <v>16</v>
@@ -823,13 +829,13 @@
         <v>7</v>
       </c>
       <c r="N9" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="O9" s="6" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A10">
         <f t="shared" si="0"/>
         <v>18</v>
@@ -860,7 +866,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A11">
         <f t="shared" si="0"/>
         <v>20</v>
@@ -891,7 +897,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A12">
         <f t="shared" si="0"/>
         <v>22</v>
@@ -922,13 +928,13 @@
         <v>7</v>
       </c>
       <c r="N12" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="O12" s="6" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A13">
         <f t="shared" si="0"/>
         <v>24</v>
@@ -959,13 +965,13 @@
         <v>13</v>
       </c>
       <c r="N13" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="O13" s="4" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A14">
         <f t="shared" si="0"/>
         <v>26</v>
@@ -996,7 +1002,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A15">
         <f t="shared" si="0"/>
         <v>28</v>
@@ -1027,7 +1033,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A16">
         <f t="shared" si="0"/>
         <v>30</v>
@@ -1058,7 +1064,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A17">
         <f t="shared" si="0"/>
         <v>32</v>
@@ -1089,7 +1095,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A18">
         <f t="shared" si="0"/>
         <v>34</v>
@@ -1120,7 +1126,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A19">
         <f t="shared" si="0"/>
         <v>36</v>
@@ -1142,7 +1148,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A20">
         <f t="shared" si="0"/>
         <v>38</v>
@@ -1165,7 +1171,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A21">
         <f t="shared" si="0"/>
         <v>40</v>
@@ -1187,7 +1193,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A22">
         <f t="shared" si="0"/>
         <v>42</v>
@@ -1208,7 +1214,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A23">
         <f t="shared" si="0"/>
         <v>44</v>
@@ -1230,7 +1236,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A24">
         <f t="shared" si="0"/>
         <v>46</v>
@@ -1252,7 +1258,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A25">
         <f>A24+2</f>
         <v>48</v>
@@ -1274,7 +1280,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
       <c r="E26">
         <f t="shared" si="2"/>
         <v>55</v>
@@ -1286,7 +1292,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
       <c r="E27">
         <f t="shared" si="2"/>
         <v>57</v>
@@ -1298,7 +1304,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
       <c r="E28">
         <f t="shared" si="2"/>
         <v>59</v>

</xml_diff>

<commit_message>
Hardware portion of lab report complete
</commit_message>
<xml_diff>
--- a/Connections_Table.xlsx
+++ b/Connections_Table.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="47">
   <si>
     <t>Expansion Board J11</t>
   </si>
@@ -162,6 +162,9 @@
   </si>
   <si>
     <t>KeyPad(5)</t>
+  </si>
+  <si>
+    <t>NOTE: ** indicates that wires of this color connect to the same pin</t>
   </si>
 </sst>
 </file>
@@ -516,23 +519,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O28"/>
+  <dimension ref="A1:O30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="A30" sqref="A30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="10.26953125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.28515625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="23" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10.453125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.42578125" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="11" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="23" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="10.453125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="10.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -546,7 +549,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -584,7 +587,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>4</v>
       </c>
@@ -617,7 +620,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4">
         <f>A3+2</f>
         <v>6</v>
@@ -657,7 +660,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5">
         <f t="shared" ref="A5:A26" si="0">A4+2</f>
         <v>8</v>
@@ -697,7 +700,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -737,7 +740,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7">
         <f t="shared" si="0"/>
         <v>12</v>
@@ -777,7 +780,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8">
         <f t="shared" si="0"/>
         <v>14</v>
@@ -817,7 +820,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9">
         <f t="shared" si="0"/>
         <v>16</v>
@@ -857,7 +860,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>17</v>
       </c>
@@ -888,7 +891,7 @@
       </c>
       <c r="O10" s="1"/>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11">
         <f>A9+2</f>
         <v>18</v>
@@ -925,7 +928,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>19</v>
       </c>
@@ -961,7 +964,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13">
         <f>A11+2</f>
         <v>20</v>
@@ -992,7 +995,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14">
         <f t="shared" si="0"/>
         <v>22</v>
@@ -1023,7 +1026,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15">
         <f t="shared" si="0"/>
         <v>24</v>
@@ -1054,7 +1057,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16">
         <f t="shared" si="0"/>
         <v>26</v>
@@ -1085,7 +1088,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17">
         <f t="shared" si="0"/>
         <v>28</v>
@@ -1116,7 +1119,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18">
         <f t="shared" si="0"/>
         <v>30</v>
@@ -1147,7 +1150,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19">
         <f t="shared" si="0"/>
         <v>32</v>
@@ -1169,7 +1172,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20">
         <f t="shared" si="0"/>
         <v>34</v>
@@ -1191,7 +1194,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21">
         <f t="shared" si="0"/>
         <v>36</v>
@@ -1213,7 +1216,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22">
         <f t="shared" si="0"/>
         <v>38</v>
@@ -1235,7 +1238,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23">
         <f t="shared" si="0"/>
         <v>40</v>
@@ -1257,7 +1260,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24">
         <f t="shared" si="0"/>
         <v>42</v>
@@ -1279,7 +1282,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25">
         <f t="shared" si="0"/>
         <v>44</v>
@@ -1301,7 +1304,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26">
         <f t="shared" si="0"/>
         <v>46</v>
@@ -1323,7 +1326,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27">
         <f>A26+2</f>
         <v>48</v>
@@ -1345,7 +1348,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="E28">
         <f t="shared" si="2"/>
         <v>59</v>
@@ -1355,6 +1358,11 @@
       </c>
       <c r="G28" t="s">
         <v>7</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>46</v>
       </c>
     </row>
   </sheetData>

</xml_diff>